<commit_message>
END OF DAY  tHURSDAY 30-jULY-21
</commit_message>
<xml_diff>
--- a/KakanuiXS Lines 1 to 18 - Copy.20210706145755948.xlsx
+++ b/KakanuiXS Lines 1 to 18 - Copy.20210706145755948.xlsx
@@ -1112,11 +1112,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1133,8 +1133,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1148,17 +1149,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1187,7 +1180,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1201,9 +1216,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1218,15 +1232,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1234,22 +1240,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1263,15 +1269,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1292,19 +1292,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1322,7 +1310,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1340,7 +1358,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1352,25 +1436,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1388,37 +1454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1430,49 +1466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1483,6 +1483,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1525,17 +1540,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1574,19 +1583,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1604,130 +1604,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2074,10 +2074,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S602"/>
+  <dimension ref="A1:S603"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164:F184"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A518" workbookViewId="0">
+      <selection activeCell="F525" sqref="C525:F526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4"/>
@@ -18630,53 +18630,24 @@
         <v>271</v>
       </c>
     </row>
-    <row r="524" spans="1:11">
-      <c r="A524" t="s">
-        <v>276</v>
-      </c>
-      <c r="B524">
-        <v>10022</v>
-      </c>
-      <c r="C524" s="7">
-        <v>6.07842907382626</v>
-      </c>
-      <c r="D524" s="7">
-        <v>50.317</v>
-      </c>
-      <c r="E524" s="7">
-        <v>1427289.83</v>
-      </c>
-      <c r="F524" s="7">
-        <v>5006048.81</v>
-      </c>
-      <c r="H524" t="s">
-        <v>11</v>
-      </c>
-      <c r="I524" t="s">
-        <v>15</v>
-      </c>
-      <c r="K524" t="s">
-        <v>277</v>
-      </c>
-    </row>
     <row r="525" spans="1:11">
       <c r="A525" t="s">
         <v>276</v>
       </c>
       <c r="B525">
-        <v>10021</v>
+        <v>10022</v>
       </c>
       <c r="C525" s="7">
-        <v>6.15958602495402</v>
+        <v>6.07842907382626</v>
       </c>
       <c r="D525" s="7">
-        <v>50.167</v>
+        <v>50.317</v>
       </c>
       <c r="E525" s="7">
-        <v>1427284.13</v>
+        <v>1427289.83</v>
       </c>
       <c r="F525" s="7">
-        <v>5006048.95</v>
+        <v>5006048.81</v>
       </c>
       <c r="H525" t="s">
         <v>11</v>
@@ -18693,19 +18664,19 @@
         <v>276</v>
       </c>
       <c r="B526">
-        <v>10023</v>
+        <v>10021</v>
       </c>
       <c r="C526" s="7">
-        <v>15.2967218706343</v>
+        <v>6.15958602495402</v>
       </c>
       <c r="D526" s="7">
-        <v>50.847</v>
+        <v>50.167</v>
       </c>
       <c r="E526" s="7">
-        <v>1427291.89</v>
+        <v>1427284.13</v>
       </c>
       <c r="F526" s="7">
-        <v>5006039.73</v>
+        <v>5006048.95</v>
       </c>
       <c r="H526" t="s">
         <v>11</v>
@@ -18722,25 +18693,25 @@
         <v>276</v>
       </c>
       <c r="B527">
-        <v>10024</v>
+        <v>10023</v>
       </c>
       <c r="C527" s="7">
-        <v>31.3970094113157</v>
+        <v>15.2967218706343</v>
       </c>
       <c r="D527" s="7">
-        <v>50.938</v>
+        <v>50.847</v>
       </c>
       <c r="E527" s="7">
-        <v>1427295.39</v>
+        <v>1427291.89</v>
       </c>
       <c r="F527" s="7">
-        <v>5006023.98</v>
+        <v>5006039.73</v>
       </c>
       <c r="H527" t="s">
         <v>11</v>
       </c>
       <c r="I527" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K527" t="s">
         <v>277</v>
@@ -18751,25 +18722,25 @@
         <v>276</v>
       </c>
       <c r="B528">
-        <v>10025</v>
+        <v>10024</v>
       </c>
       <c r="C528" s="7">
-        <v>33.0408671195925</v>
+        <v>31.3970094113157</v>
       </c>
       <c r="D528" s="7">
-        <v>49.738</v>
+        <v>50.938</v>
       </c>
       <c r="E528" s="7">
-        <v>1427295.62</v>
+        <v>1427295.39</v>
       </c>
       <c r="F528" s="7">
-        <v>5006022.34</v>
+        <v>5006023.98</v>
       </c>
       <c r="H528" t="s">
         <v>11</v>
       </c>
       <c r="I528" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K528" t="s">
         <v>277</v>
@@ -18780,25 +18751,25 @@
         <v>276</v>
       </c>
       <c r="B529">
-        <v>10026</v>
+        <v>10025</v>
       </c>
       <c r="C529" s="7">
-        <v>44.6442314302917</v>
+        <v>33.0408671195925</v>
       </c>
       <c r="D529" s="7">
-        <v>49.628</v>
+        <v>49.738</v>
       </c>
       <c r="E529" s="7">
-        <v>1427298.27</v>
+        <v>1427295.62</v>
       </c>
       <c r="F529" s="7">
-        <v>5006011.04</v>
+        <v>5006022.34</v>
       </c>
       <c r="H529" t="s">
         <v>11</v>
       </c>
       <c r="I529" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K529" t="s">
         <v>277</v>
@@ -18809,19 +18780,19 @@
         <v>276</v>
       </c>
       <c r="B530">
-        <v>10027</v>
+        <v>10026</v>
       </c>
       <c r="C530" s="7">
-        <v>54.9740029472095</v>
+        <v>44.6442314302917</v>
       </c>
       <c r="D530" s="7">
-        <v>49.789</v>
+        <v>49.628</v>
       </c>
       <c r="E530" s="7">
-        <v>1427299.37</v>
+        <v>1427298.27</v>
       </c>
       <c r="F530" s="7">
-        <v>5006000.68</v>
+        <v>5006011.04</v>
       </c>
       <c r="H530" t="s">
         <v>11</v>
@@ -18838,19 +18809,19 @@
         <v>276</v>
       </c>
       <c r="B531">
-        <v>10028</v>
+        <v>10027</v>
       </c>
       <c r="C531" s="7">
-        <v>55.1775969030918</v>
+        <v>54.9740029472095</v>
       </c>
       <c r="D531" s="7">
-        <v>49.759</v>
+        <v>49.789</v>
       </c>
       <c r="E531" s="7">
-        <v>1427300.86</v>
+        <v>1427299.37</v>
       </c>
       <c r="F531" s="7">
-        <v>5006000.83</v>
+        <v>5006000.68</v>
       </c>
       <c r="H531" t="s">
         <v>11</v>
@@ -18867,19 +18838,19 @@
         <v>276</v>
       </c>
       <c r="B532">
-        <v>10029</v>
+        <v>10028</v>
       </c>
       <c r="C532" s="7">
-        <v>66.7409536940992</v>
+        <v>55.1775969030918</v>
       </c>
       <c r="D532" s="7">
-        <v>50.349</v>
+        <v>49.759</v>
       </c>
       <c r="E532" s="7">
-        <v>1427303.38</v>
+        <v>1427300.86</v>
       </c>
       <c r="F532" s="7">
-        <v>5005989.54</v>
+        <v>5006000.83</v>
       </c>
       <c r="H532" t="s">
         <v>11</v>
@@ -18896,19 +18867,19 @@
         <v>276</v>
       </c>
       <c r="B533">
-        <v>10030</v>
+        <v>10029</v>
       </c>
       <c r="C533" s="7">
-        <v>77.1214918165923</v>
+        <v>66.7409536940992</v>
       </c>
       <c r="D533" s="7">
-        <v>49.99</v>
+        <v>50.349</v>
       </c>
       <c r="E533" s="7">
-        <v>1427305.86</v>
+        <v>1427303.38</v>
       </c>
       <c r="F533" s="7">
-        <v>5005979.46</v>
+        <v>5005989.54</v>
       </c>
       <c r="H533" t="s">
         <v>11</v>
@@ -18925,28 +18896,25 @@
         <v>276</v>
       </c>
       <c r="B534">
-        <v>10031</v>
+        <v>10030</v>
       </c>
       <c r="C534" s="7">
-        <v>86.8471582724682</v>
+        <v>77.1214918165923</v>
       </c>
       <c r="D534" s="7">
-        <v>49.32</v>
+        <v>49.99</v>
       </c>
       <c r="E534" s="7">
-        <v>1427308.28</v>
+        <v>1427305.86</v>
       </c>
       <c r="F534" s="7">
-        <v>5005970.04</v>
+        <v>5005979.46</v>
       </c>
       <c r="H534" t="s">
         <v>11</v>
       </c>
       <c r="I534" t="s">
-        <v>19</v>
-      </c>
-      <c r="J534" s="8" t="s">
-        <v>278</v>
+        <v>15</v>
       </c>
       <c r="K534" t="s">
         <v>277</v>
@@ -18957,25 +18925,28 @@
         <v>276</v>
       </c>
       <c r="B535">
-        <v>10032</v>
+        <v>10031</v>
       </c>
       <c r="C535" s="7">
-        <v>90.0571068827097</v>
+        <v>86.8471582724682</v>
       </c>
       <c r="D535" s="7">
-        <v>49.1</v>
+        <v>49.32</v>
       </c>
       <c r="E535" s="7">
-        <v>1427308.59</v>
+        <v>1427308.28</v>
       </c>
       <c r="F535" s="7">
-        <v>5005966.81</v>
+        <v>5005970.04</v>
       </c>
       <c r="H535" t="s">
         <v>11</v>
       </c>
       <c r="I535" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J535" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="K535" t="s">
         <v>277</v>
@@ -18986,19 +18957,19 @@
         <v>276</v>
       </c>
       <c r="B536">
-        <v>10033</v>
+        <v>10032</v>
       </c>
       <c r="C536" s="7">
-        <v>95.0723818993767</v>
+        <v>90.0571068827097</v>
       </c>
       <c r="D536" s="7">
-        <v>48.98</v>
+        <v>49.1</v>
       </c>
       <c r="E536" s="7">
-        <v>1427309.87</v>
+        <v>1427308.59</v>
       </c>
       <c r="F536" s="7">
-        <v>5005961.96</v>
+        <v>5005966.81</v>
       </c>
       <c r="H536" t="s">
         <v>11</v>
@@ -19015,19 +18986,19 @@
         <v>276</v>
       </c>
       <c r="B537">
-        <v>10034</v>
+        <v>10033</v>
       </c>
       <c r="C537" s="7">
-        <v>99.2552794566151</v>
+        <v>95.0723818993767</v>
       </c>
       <c r="D537" s="7">
-        <v>48.67</v>
+        <v>48.98</v>
       </c>
       <c r="E537" s="7">
-        <v>1427311.28</v>
+        <v>1427309.87</v>
       </c>
       <c r="F537" s="7">
-        <v>5005958</v>
+        <v>5005961.96</v>
       </c>
       <c r="H537" t="s">
         <v>11</v>
@@ -19044,19 +19015,19 @@
         <v>276</v>
       </c>
       <c r="B538">
-        <v>10036</v>
+        <v>10034</v>
       </c>
       <c r="C538" s="7">
-        <v>101.747955753028</v>
+        <v>99.2552794566151</v>
       </c>
       <c r="D538" s="7">
-        <v>48.94</v>
+        <v>48.67</v>
       </c>
       <c r="E538" s="7">
-        <v>1427312.47</v>
+        <v>1427311.28</v>
       </c>
       <c r="F538" s="7">
-        <v>5005955.73</v>
+        <v>5005958</v>
       </c>
       <c r="H538" t="s">
         <v>11</v>
@@ -19073,28 +19044,25 @@
         <v>276</v>
       </c>
       <c r="B539">
-        <v>10035</v>
+        <v>10036</v>
       </c>
       <c r="C539" s="7">
-        <v>101.892465864779</v>
+        <v>101.747955753028</v>
       </c>
       <c r="D539" s="7">
-        <v>49.18</v>
+        <v>48.94</v>
       </c>
       <c r="E539" s="7">
-        <v>1427312.31</v>
+        <v>1427312.47</v>
       </c>
       <c r="F539" s="7">
-        <v>5005955.54</v>
+        <v>5005955.73</v>
       </c>
       <c r="H539" t="s">
         <v>11</v>
       </c>
       <c r="I539" t="s">
-        <v>19</v>
-      </c>
-      <c r="J539" s="8" t="s">
-        <v>279</v>
+        <v>15</v>
       </c>
       <c r="K539" t="s">
         <v>277</v>
@@ -19105,25 +19073,28 @@
         <v>276</v>
       </c>
       <c r="B540">
-        <v>10037</v>
+        <v>10035</v>
       </c>
       <c r="C540" s="7">
-        <v>104.714753975168</v>
+        <v>101.892465864779</v>
       </c>
       <c r="D540" s="7">
-        <v>51.241</v>
+        <v>49.18</v>
       </c>
       <c r="E540" s="7">
-        <v>1427314.14</v>
+        <v>1427312.31</v>
       </c>
       <c r="F540" s="7">
-        <v>5005953.1</v>
+        <v>5005955.54</v>
       </c>
       <c r="H540" t="s">
         <v>11</v>
       </c>
       <c r="I540" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J540" s="8" t="s">
+        <v>279</v>
       </c>
       <c r="K540" t="s">
         <v>277</v>
@@ -19134,19 +19105,19 @@
         <v>276</v>
       </c>
       <c r="B541">
-        <v>10038</v>
+        <v>10037</v>
       </c>
       <c r="C541" s="7">
-        <v>150.31510270078</v>
+        <v>104.714753975168</v>
       </c>
       <c r="D541" s="7">
-        <v>50.262</v>
+        <v>51.241</v>
       </c>
       <c r="E541" s="7">
-        <v>1427321.71</v>
+        <v>1427314.14</v>
       </c>
       <c r="F541" s="7">
-        <v>5005907.99</v>
+        <v>5005953.1</v>
       </c>
       <c r="H541" t="s">
         <v>11</v>
@@ -19163,19 +19134,19 @@
         <v>276</v>
       </c>
       <c r="B542">
-        <v>10040</v>
+        <v>10038</v>
       </c>
       <c r="C542" s="7">
-        <v>171.390072057987</v>
+        <v>150.31510270078</v>
       </c>
       <c r="D542" s="7">
-        <v>51.073</v>
+        <v>50.262</v>
       </c>
       <c r="E542" s="7">
-        <v>1427320.52</v>
+        <v>1427321.71</v>
       </c>
       <c r="F542" s="7">
-        <v>5005886.17</v>
+        <v>5005907.99</v>
       </c>
       <c r="H542" t="s">
         <v>11</v>
@@ -19192,19 +19163,19 @@
         <v>276</v>
       </c>
       <c r="B543">
-        <v>10039</v>
+        <v>10040</v>
       </c>
       <c r="C543" s="7">
-        <v>171.69970588196</v>
+        <v>171.390072057987</v>
       </c>
       <c r="D543" s="7">
-        <v>52.573</v>
+        <v>51.073</v>
       </c>
       <c r="E543" s="7">
-        <v>1427319.73</v>
+        <v>1427320.52</v>
       </c>
       <c r="F543" s="7">
-        <v>5005885.7</v>
+        <v>5005886.17</v>
       </c>
       <c r="H543" t="s">
         <v>11</v>
@@ -19218,22 +19189,22 @@
     </row>
     <row r="544" spans="1:11">
       <c r="A544" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B544">
-        <v>9058</v>
+        <v>10039</v>
       </c>
       <c r="C544" s="7">
-        <v>-1.20329755264473</v>
+        <v>171.69970588196</v>
       </c>
       <c r="D544" s="7">
-        <v>50.972</v>
+        <v>52.573</v>
       </c>
       <c r="E544" s="7">
-        <v>1427583.44</v>
+        <v>1427319.73</v>
       </c>
       <c r="F544" s="7">
-        <v>5005957.71</v>
+        <v>5005885.7</v>
       </c>
       <c r="H544" t="s">
         <v>11</v>
@@ -19242,7 +19213,7 @@
         <v>15</v>
       </c>
       <c r="K544" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="545" spans="1:11">
@@ -19250,19 +19221,19 @@
         <v>280</v>
       </c>
       <c r="B545">
-        <v>9057</v>
+        <v>9058</v>
       </c>
       <c r="C545" s="7">
-        <v>3.01307235222457</v>
+        <v>-1.20329755264473</v>
       </c>
       <c r="D545" s="7">
-        <v>51.102</v>
+        <v>50.972</v>
       </c>
       <c r="E545" s="7">
-        <v>1427582.02</v>
+        <v>1427583.44</v>
       </c>
       <c r="F545" s="7">
-        <v>5005954.58</v>
+        <v>5005957.71</v>
       </c>
       <c r="H545" t="s">
         <v>11</v>
@@ -19279,25 +19250,25 @@
         <v>280</v>
       </c>
       <c r="B546">
-        <v>9056</v>
+        <v>9057</v>
       </c>
       <c r="C546" s="7">
-        <v>6.29713943012242</v>
+        <v>3.01307235222457</v>
       </c>
       <c r="D546" s="7">
-        <v>51.482</v>
+        <v>51.102</v>
       </c>
       <c r="E546" s="7">
-        <v>1427581.08</v>
+        <v>1427582.02</v>
       </c>
       <c r="F546" s="7">
-        <v>5005951.22</v>
+        <v>5005954.58</v>
       </c>
       <c r="H546" t="s">
         <v>11</v>
       </c>
       <c r="I546" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K546" t="s">
         <v>281</v>
@@ -19308,25 +19279,25 @@
         <v>280</v>
       </c>
       <c r="B547">
-        <v>9055</v>
+        <v>9056</v>
       </c>
       <c r="C547" s="7">
-        <v>9.01308853846222</v>
+        <v>6.29713943012242</v>
       </c>
       <c r="D547" s="7">
-        <v>52.672</v>
+        <v>51.482</v>
       </c>
       <c r="E547" s="7">
-        <v>1427579.7</v>
+        <v>1427581.08</v>
       </c>
       <c r="F547" s="7">
-        <v>5005948.88</v>
+        <v>5005951.22</v>
       </c>
       <c r="H547" t="s">
         <v>11</v>
       </c>
       <c r="I547" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K547" t="s">
         <v>281</v>
@@ -19337,19 +19308,19 @@
         <v>280</v>
       </c>
       <c r="B548">
-        <v>9054</v>
+        <v>9055</v>
       </c>
       <c r="C548" s="7">
-        <v>10.2863727814426</v>
+        <v>9.01308853846222</v>
       </c>
       <c r="D548" s="7">
-        <v>52.832</v>
+        <v>52.672</v>
       </c>
       <c r="E548" s="7">
-        <v>1427579.95</v>
+        <v>1427579.7</v>
       </c>
       <c r="F548" s="7">
-        <v>5005947.33</v>
+        <v>5005948.88</v>
       </c>
       <c r="H548" t="s">
         <v>11</v>
@@ -19366,25 +19337,25 @@
         <v>280</v>
       </c>
       <c r="B549">
-        <v>9053</v>
+        <v>9054</v>
       </c>
       <c r="C549" s="7">
-        <v>15.5352156407307</v>
+        <v>10.2863727814426</v>
       </c>
       <c r="D549" s="7">
-        <v>49.742</v>
+        <v>52.832</v>
       </c>
       <c r="E549" s="7">
-        <v>1427576.32</v>
+        <v>1427579.95</v>
       </c>
       <c r="F549" s="7">
-        <v>5005943.3</v>
+        <v>5005947.33</v>
       </c>
       <c r="H549" t="s">
         <v>11</v>
       </c>
       <c r="I549" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K549" t="s">
         <v>281</v>
@@ -19395,25 +19366,25 @@
         <v>280</v>
       </c>
       <c r="B550">
-        <v>9052</v>
+        <v>9053</v>
       </c>
       <c r="C550" s="7">
-        <v>18.3587179565716</v>
+        <v>15.5352156407307</v>
       </c>
       <c r="D550" s="7">
-        <v>49.212</v>
+        <v>49.742</v>
       </c>
       <c r="E550" s="7">
-        <v>1427574.78</v>
+        <v>1427576.32</v>
       </c>
       <c r="F550" s="7">
-        <v>5005940.93</v>
+        <v>5005943.3</v>
       </c>
       <c r="H550" t="s">
         <v>11</v>
       </c>
       <c r="I550" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K550" t="s">
         <v>281</v>
@@ -19424,19 +19395,19 @@
         <v>280</v>
       </c>
       <c r="B551">
-        <v>9051</v>
+        <v>9052</v>
       </c>
       <c r="C551" s="7">
-        <v>19.5436927166857</v>
+        <v>18.3587179565716</v>
       </c>
       <c r="D551" s="7">
-        <v>48.702</v>
+        <v>49.212</v>
       </c>
       <c r="E551" s="7">
-        <v>1427574.16</v>
+        <v>1427574.78</v>
       </c>
       <c r="F551" s="7">
-        <v>5005939.92</v>
+        <v>5005940.93</v>
       </c>
       <c r="H551" t="s">
         <v>11</v>
@@ -19453,28 +19424,25 @@
         <v>280</v>
       </c>
       <c r="B552">
-        <v>9050</v>
+        <v>9051</v>
       </c>
       <c r="C552" s="7">
-        <v>20.402071096235</v>
+        <v>19.5436927166857</v>
       </c>
       <c r="D552" s="7">
-        <v>48.172</v>
+        <v>48.702</v>
       </c>
       <c r="E552" s="7">
-        <v>1427573.93</v>
+        <v>1427574.16</v>
       </c>
       <c r="F552" s="7">
-        <v>5005939.06</v>
+        <v>5005939.92</v>
       </c>
       <c r="H552" t="s">
         <v>11</v>
       </c>
       <c r="I552" t="s">
-        <v>19</v>
-      </c>
-      <c r="J552" s="8" t="s">
-        <v>282</v>
+        <v>15</v>
       </c>
       <c r="K552" t="s">
         <v>281</v>
@@ -19485,25 +19453,28 @@
         <v>280</v>
       </c>
       <c r="B553">
-        <v>9049</v>
+        <v>9050</v>
       </c>
       <c r="C553" s="7">
-        <v>20.9117867478853</v>
+        <v>20.402071096235</v>
       </c>
       <c r="D553" s="7">
-        <v>47.162</v>
+        <v>48.172</v>
       </c>
       <c r="E553" s="7">
-        <v>1427573.69</v>
+        <v>1427573.93</v>
       </c>
       <c r="F553" s="7">
-        <v>5005938.61</v>
+        <v>5005939.06</v>
       </c>
       <c r="H553" t="s">
         <v>11</v>
       </c>
       <c r="I553" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J553" s="8" t="s">
+        <v>282</v>
       </c>
       <c r="K553" t="s">
         <v>281</v>
@@ -19514,19 +19485,19 @@
         <v>280</v>
       </c>
       <c r="B554">
-        <v>9048</v>
+        <v>9049</v>
       </c>
       <c r="C554" s="7">
-        <v>30.1798784786996</v>
+        <v>20.9117867478853</v>
       </c>
       <c r="D554" s="7">
-        <v>46.882</v>
+        <v>47.162</v>
       </c>
       <c r="E554" s="7">
-        <v>1427569.29</v>
+        <v>1427573.69</v>
       </c>
       <c r="F554" s="7">
-        <v>5005930.45</v>
+        <v>5005938.61</v>
       </c>
       <c r="H554" t="s">
         <v>11</v>
@@ -19543,19 +19514,19 @@
         <v>280</v>
       </c>
       <c r="B555">
-        <v>9047</v>
+        <v>9048</v>
       </c>
       <c r="C555" s="7">
-        <v>33.7012727507173</v>
+        <v>30.1798784786996</v>
       </c>
       <c r="D555" s="7">
-        <v>47.302</v>
+        <v>46.882</v>
       </c>
       <c r="E555" s="7">
-        <v>1427566.35</v>
+        <v>1427569.29</v>
       </c>
       <c r="F555" s="7">
-        <v>5005928.1</v>
+        <v>5005930.45</v>
       </c>
       <c r="H555" t="s">
         <v>11</v>
@@ -19572,19 +19543,19 @@
         <v>280</v>
       </c>
       <c r="B556">
-        <v>9046</v>
+        <v>9047</v>
       </c>
       <c r="C556" s="7">
-        <v>35.9558908248721</v>
+        <v>33.7012727507173</v>
       </c>
       <c r="D556" s="7">
-        <v>47.432</v>
+        <v>47.302</v>
       </c>
       <c r="E556" s="7">
-        <v>1427565.66</v>
+        <v>1427566.35</v>
       </c>
       <c r="F556" s="7">
-        <v>5005925.88</v>
+        <v>5005928.1</v>
       </c>
       <c r="H556" t="s">
         <v>11</v>
@@ -19601,19 +19572,19 @@
         <v>280</v>
       </c>
       <c r="B557">
-        <v>9045</v>
+        <v>9046</v>
       </c>
       <c r="C557" s="7">
-        <v>38.9647790318104</v>
+        <v>35.9558908248721</v>
       </c>
       <c r="D557" s="7">
-        <v>47.202</v>
+        <v>47.432</v>
       </c>
       <c r="E557" s="7">
-        <v>1427565.06</v>
+        <v>1427565.66</v>
       </c>
       <c r="F557" s="7">
-        <v>5005922.75</v>
+        <v>5005925.88</v>
       </c>
       <c r="H557" t="s">
         <v>11</v>
@@ -19630,19 +19601,19 @@
         <v>280</v>
       </c>
       <c r="B558">
-        <v>9044</v>
+        <v>9045</v>
       </c>
       <c r="C558" s="7">
-        <v>44.2618495430203</v>
+        <v>38.9647790318104</v>
       </c>
       <c r="D558" s="7">
-        <v>47.262</v>
+        <v>47.202</v>
       </c>
       <c r="E558" s="7">
-        <v>1427561.5</v>
+        <v>1427565.06</v>
       </c>
       <c r="F558" s="7">
-        <v>5005918.69</v>
+        <v>5005922.75</v>
       </c>
       <c r="H558" t="s">
         <v>11</v>
@@ -19659,19 +19630,19 @@
         <v>280</v>
       </c>
       <c r="B559">
-        <v>9043</v>
+        <v>9044</v>
       </c>
       <c r="C559" s="7">
-        <v>47.6761821566449</v>
+        <v>44.2618495430203</v>
       </c>
       <c r="D559" s="7">
-        <v>47.412</v>
+        <v>47.262</v>
       </c>
       <c r="E559" s="7">
-        <v>1427559.25</v>
+        <v>1427561.5</v>
       </c>
       <c r="F559" s="7">
-        <v>5005916.06</v>
+        <v>5005918.69</v>
       </c>
       <c r="H559" t="s">
         <v>11</v>
@@ -19688,19 +19659,19 @@
         <v>280</v>
       </c>
       <c r="B560">
-        <v>9042</v>
+        <v>9043</v>
       </c>
       <c r="C560" s="7">
-        <v>51.633735145129</v>
+        <v>47.6761821566449</v>
       </c>
       <c r="D560" s="7">
-        <v>47.672</v>
+        <v>47.412</v>
       </c>
       <c r="E560" s="7">
-        <v>1427556.98</v>
+        <v>1427559.25</v>
       </c>
       <c r="F560" s="7">
-        <v>5005912.81</v>
+        <v>5005916.06</v>
       </c>
       <c r="H560" t="s">
         <v>11</v>
@@ -19717,19 +19688,19 @@
         <v>280</v>
       </c>
       <c r="B561">
-        <v>9041</v>
+        <v>9042</v>
       </c>
       <c r="C561" s="7">
-        <v>56.9772072413341</v>
+        <v>51.633735145129</v>
       </c>
       <c r="D561" s="7">
-        <v>47.792</v>
+        <v>47.672</v>
       </c>
       <c r="E561" s="7">
-        <v>1427555.07</v>
+        <v>1427556.98</v>
       </c>
       <c r="F561" s="7">
-        <v>5005907.72</v>
+        <v>5005912.81</v>
       </c>
       <c r="H561" t="s">
         <v>11</v>
@@ -19746,19 +19717,19 @@
         <v>280</v>
       </c>
       <c r="B562">
-        <v>9040</v>
+        <v>9041</v>
       </c>
       <c r="C562" s="7">
-        <v>59.677701405004</v>
+        <v>56.9772072413341</v>
       </c>
       <c r="D562" s="7">
-        <v>47.932</v>
+        <v>47.792</v>
       </c>
       <c r="E562" s="7">
-        <v>1427553.32</v>
+        <v>1427555.07</v>
       </c>
       <c r="F562" s="7">
-        <v>5005905.62</v>
+        <v>5005907.72</v>
       </c>
       <c r="H562" t="s">
         <v>11</v>
@@ -19775,28 +19746,25 @@
         <v>280</v>
       </c>
       <c r="B563">
-        <v>9039</v>
+        <v>9040</v>
       </c>
       <c r="C563" s="7">
-        <v>60.3002154638935</v>
+        <v>59.677701405004</v>
       </c>
       <c r="D563" s="7">
-        <v>48.142</v>
+        <v>47.932</v>
       </c>
       <c r="E563" s="7">
-        <v>1427553.01</v>
+        <v>1427553.32</v>
       </c>
       <c r="F563" s="7">
-        <v>5005905.08</v>
+        <v>5005905.62</v>
       </c>
       <c r="H563" t="s">
         <v>11</v>
       </c>
       <c r="I563" t="s">
-        <v>19</v>
-      </c>
-      <c r="J563" s="8" t="s">
-        <v>283</v>
+        <v>15</v>
       </c>
       <c r="K563" t="s">
         <v>281</v>
@@ -19807,25 +19775,28 @@
         <v>280</v>
       </c>
       <c r="B564">
-        <v>9038</v>
+        <v>9039</v>
       </c>
       <c r="C564" s="7">
-        <v>60.5061342759949</v>
+        <v>60.3002154638935</v>
       </c>
       <c r="D564" s="7">
-        <v>48.192</v>
+        <v>48.142</v>
       </c>
       <c r="E564" s="7">
-        <v>1427552.86</v>
+        <v>1427553.01</v>
       </c>
       <c r="F564" s="7">
-        <v>5005904.93</v>
+        <v>5005905.08</v>
       </c>
       <c r="H564" t="s">
         <v>11</v>
       </c>
       <c r="I564" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J564" s="8" t="s">
+        <v>283</v>
       </c>
       <c r="K564" t="s">
         <v>281</v>
@@ -19836,19 +19807,19 @@
         <v>280</v>
       </c>
       <c r="B565">
-        <v>9037</v>
+        <v>9038</v>
       </c>
       <c r="C565" s="7">
-        <v>63.3770390993488</v>
+        <v>60.5061342759949</v>
       </c>
       <c r="D565" s="7">
-        <v>48.652</v>
+        <v>48.192</v>
       </c>
       <c r="E565" s="7">
-        <v>1427551.68</v>
+        <v>1427552.86</v>
       </c>
       <c r="F565" s="7">
-        <v>5005902.29</v>
+        <v>5005904.93</v>
       </c>
       <c r="H565" t="s">
         <v>11</v>
@@ -19865,19 +19836,19 @@
         <v>280</v>
       </c>
       <c r="B566">
-        <v>9036</v>
+        <v>9037</v>
       </c>
       <c r="C566" s="7">
-        <v>67.9086726788405</v>
+        <v>63.3770390993488</v>
       </c>
       <c r="D566" s="7">
-        <v>49.202</v>
+        <v>48.652</v>
       </c>
       <c r="E566" s="7">
-        <v>1427550.61</v>
+        <v>1427551.68</v>
       </c>
       <c r="F566" s="7">
-        <v>5005897.67</v>
+        <v>5005902.29</v>
       </c>
       <c r="H566" t="s">
         <v>11</v>
@@ -19894,25 +19865,25 @@
         <v>280</v>
       </c>
       <c r="B567">
-        <v>9035</v>
+        <v>9036</v>
       </c>
       <c r="C567" s="7">
-        <v>68.6568987425946</v>
+        <v>67.9086726788405</v>
       </c>
       <c r="D567" s="7">
-        <v>48.762</v>
+        <v>49.202</v>
       </c>
       <c r="E567" s="7">
-        <v>1427549.51</v>
+        <v>1427550.61</v>
       </c>
       <c r="F567" s="7">
-        <v>5005897.44</v>
+        <v>5005897.67</v>
       </c>
       <c r="H567" t="s">
         <v>11</v>
       </c>
       <c r="I567" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K567" t="s">
         <v>281</v>
@@ -19923,25 +19894,25 @@
         <v>280</v>
       </c>
       <c r="B568">
-        <v>9034</v>
+        <v>9035</v>
       </c>
       <c r="C568" s="7">
-        <v>74.0801938779348</v>
+        <v>68.6568987425946</v>
       </c>
       <c r="D568" s="7">
-        <v>51.652</v>
+        <v>48.762</v>
       </c>
       <c r="E568" s="7">
-        <v>1427546.16</v>
+        <v>1427549.51</v>
       </c>
       <c r="F568" s="7">
-        <v>5005893.12</v>
+        <v>5005897.44</v>
       </c>
       <c r="H568" t="s">
         <v>11</v>
       </c>
       <c r="I568" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K568" t="s">
         <v>281</v>
@@ -19952,19 +19923,19 @@
         <v>280</v>
       </c>
       <c r="B569">
-        <v>9033</v>
+        <v>9034</v>
       </c>
       <c r="C569" s="7">
-        <v>75.563848267914</v>
+        <v>74.0801938779348</v>
       </c>
       <c r="D569" s="7">
-        <v>51.672</v>
+        <v>51.652</v>
       </c>
       <c r="E569" s="7">
-        <v>1427545.46</v>
+        <v>1427546.16</v>
       </c>
       <c r="F569" s="7">
-        <v>5005891.81</v>
+        <v>5005893.12</v>
       </c>
       <c r="H569" t="s">
         <v>11</v>
@@ -19981,25 +19952,25 @@
         <v>280</v>
       </c>
       <c r="B570">
-        <v>9032</v>
+        <v>9033</v>
       </c>
       <c r="C570" s="7">
-        <v>79.3350114701957</v>
+        <v>75.563848267914</v>
       </c>
       <c r="D570" s="7">
-        <v>49.722</v>
+        <v>51.672</v>
       </c>
       <c r="E570" s="7">
-        <v>1427543.8</v>
+        <v>1427545.46</v>
       </c>
       <c r="F570" s="7">
-        <v>5005888.41</v>
+        <v>5005891.81</v>
       </c>
       <c r="H570" t="s">
         <v>11</v>
       </c>
       <c r="I570" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K570" t="s">
         <v>281</v>
@@ -20010,25 +19981,25 @@
         <v>280</v>
       </c>
       <c r="B571">
-        <v>9031</v>
+        <v>9032</v>
       </c>
       <c r="C571" s="7">
-        <v>80.7814788488449</v>
+        <v>79.3350114701957</v>
       </c>
       <c r="D571" s="7">
-        <v>49.382</v>
+        <v>49.722</v>
       </c>
       <c r="E571" s="7">
-        <v>1427542.92</v>
+        <v>1427543.8</v>
       </c>
       <c r="F571" s="7">
-        <v>5005887.25</v>
+        <v>5005888.41</v>
       </c>
       <c r="H571" t="s">
         <v>11</v>
       </c>
       <c r="I571" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K571" t="s">
         <v>281</v>
@@ -20039,19 +20010,19 @@
         <v>280</v>
       </c>
       <c r="B572">
-        <v>9030</v>
+        <v>9031</v>
       </c>
       <c r="C572" s="7">
-        <v>84.228806266161</v>
+        <v>80.7814788488449</v>
       </c>
       <c r="D572" s="7">
         <v>49.382</v>
       </c>
       <c r="E572" s="7">
-        <v>1427541.56</v>
+        <v>1427542.92</v>
       </c>
       <c r="F572" s="7">
-        <v>5005884.05</v>
+        <v>5005887.25</v>
       </c>
       <c r="H572" t="s">
         <v>11</v>
@@ -20068,19 +20039,19 @@
         <v>280</v>
       </c>
       <c r="B573">
-        <v>9029</v>
+        <v>9030</v>
       </c>
       <c r="C573" s="7">
-        <v>89.4138950331693</v>
+        <v>84.228806266161</v>
       </c>
       <c r="D573" s="7">
-        <v>49.462</v>
+        <v>49.382</v>
       </c>
       <c r="E573" s="7">
-        <v>1427538.29</v>
+        <v>1427541.56</v>
       </c>
       <c r="F573" s="7">
-        <v>5005879.96</v>
+        <v>5005884.05</v>
       </c>
       <c r="H573" t="s">
         <v>11</v>
@@ -20097,19 +20068,19 @@
         <v>280</v>
       </c>
       <c r="B574">
-        <v>9028</v>
+        <v>9029</v>
       </c>
       <c r="C574" s="7">
-        <v>94.4442674012937</v>
+        <v>89.4138950331693</v>
       </c>
       <c r="D574" s="7">
-        <v>48.692</v>
+        <v>49.462</v>
       </c>
       <c r="E574" s="7">
-        <v>1427536.1</v>
+        <v>1427538.29</v>
       </c>
       <c r="F574" s="7">
-        <v>5005875.41</v>
+        <v>5005879.96</v>
       </c>
       <c r="H574" t="s">
         <v>11</v>
@@ -20126,19 +20097,19 @@
         <v>280</v>
       </c>
       <c r="B575">
-        <v>9027</v>
+        <v>9028</v>
       </c>
       <c r="C575" s="7">
-        <v>99.1054356982094</v>
+        <v>94.4442674012937</v>
       </c>
       <c r="D575" s="7">
         <v>48.692</v>
       </c>
       <c r="E575" s="7">
-        <v>1427533.37</v>
+        <v>1427536.1</v>
       </c>
       <c r="F575" s="7">
-        <v>5005871.61</v>
+        <v>5005875.41</v>
       </c>
       <c r="H575" t="s">
         <v>11</v>
@@ -20155,19 +20126,19 @@
         <v>280</v>
       </c>
       <c r="B576">
-        <v>9026</v>
+        <v>9027</v>
       </c>
       <c r="C576" s="7">
-        <v>107.906396404184</v>
+        <v>99.1054356982094</v>
       </c>
       <c r="D576" s="7">
-        <v>48.672</v>
+        <v>48.692</v>
       </c>
       <c r="E576" s="7">
-        <v>1427528.63</v>
+        <v>1427533.37</v>
       </c>
       <c r="F576" s="7">
-        <v>5005864.19</v>
+        <v>5005871.61</v>
       </c>
       <c r="H576" t="s">
         <v>11</v>
@@ -20184,19 +20155,19 @@
         <v>280</v>
       </c>
       <c r="B577">
-        <v>9025</v>
+        <v>9026</v>
       </c>
       <c r="C577" s="7">
-        <v>112.233926711153</v>
+        <v>107.906396404184</v>
       </c>
       <c r="D577" s="7">
-        <v>48.702</v>
+        <v>48.672</v>
       </c>
       <c r="E577" s="7">
-        <v>1427527.21</v>
+        <v>1427528.63</v>
       </c>
       <c r="F577" s="7">
-        <v>5005860</v>
+        <v>5005864.19</v>
       </c>
       <c r="H577" t="s">
         <v>11</v>
@@ -20213,19 +20184,19 @@
         <v>280</v>
       </c>
       <c r="B578">
-        <v>9024</v>
+        <v>9025</v>
       </c>
       <c r="C578" s="7">
-        <v>124.513695491341</v>
+        <v>112.233926711153</v>
       </c>
       <c r="D578" s="7">
-        <v>48.792</v>
+        <v>48.702</v>
       </c>
       <c r="E578" s="7">
-        <v>1427520.52</v>
+        <v>1427527.21</v>
       </c>
       <c r="F578" s="7">
-        <v>5005849.69</v>
+        <v>5005860</v>
       </c>
       <c r="H578" t="s">
         <v>11</v>
@@ -20242,19 +20213,19 @@
         <v>280</v>
       </c>
       <c r="B579">
-        <v>9023</v>
+        <v>9024</v>
       </c>
       <c r="C579" s="7">
-        <v>133.563925463002</v>
+        <v>124.513695491341</v>
       </c>
       <c r="D579" s="7">
-        <v>48.732</v>
+        <v>48.792</v>
       </c>
       <c r="E579" s="7">
-        <v>1427515.93</v>
+        <v>1427520.52</v>
       </c>
       <c r="F579" s="7">
-        <v>5005841.89</v>
+        <v>5005849.69</v>
       </c>
       <c r="H579" t="s">
         <v>11</v>
@@ -20271,19 +20242,19 @@
         <v>280</v>
       </c>
       <c r="B580">
-        <v>9022</v>
+        <v>9023</v>
       </c>
       <c r="C580" s="7">
-        <v>138.454135889798</v>
+        <v>133.563925463002</v>
       </c>
       <c r="D580" s="7">
-        <v>48.602</v>
+        <v>48.732</v>
       </c>
       <c r="E580" s="7">
-        <v>1427513.19</v>
+        <v>1427515.93</v>
       </c>
       <c r="F580" s="7">
-        <v>5005837.83</v>
+        <v>5005841.89</v>
       </c>
       <c r="H580" t="s">
         <v>11</v>
@@ -20300,19 +20271,19 @@
         <v>280</v>
       </c>
       <c r="B581">
-        <v>9021</v>
+        <v>9022</v>
       </c>
       <c r="C581" s="7">
-        <v>146.876444078272</v>
+        <v>138.454135889798</v>
       </c>
       <c r="D581" s="7">
-        <v>48.722</v>
+        <v>48.602</v>
       </c>
       <c r="E581" s="7">
-        <v>1427508.87</v>
+        <v>1427513.19</v>
       </c>
       <c r="F581" s="7">
-        <v>5005830.6</v>
+        <v>5005837.83</v>
       </c>
       <c r="H581" t="s">
         <v>11</v>
@@ -20329,19 +20300,19 @@
         <v>280</v>
       </c>
       <c r="B582">
-        <v>9020</v>
+        <v>9021</v>
       </c>
       <c r="C582" s="7">
-        <v>151.630709636953</v>
+        <v>146.876444078272</v>
       </c>
       <c r="D582" s="7">
-        <v>48.682</v>
+        <v>48.722</v>
       </c>
       <c r="E582" s="7">
-        <v>1427506.53</v>
+        <v>1427508.87</v>
       </c>
       <c r="F582" s="7">
-        <v>5005826.46</v>
+        <v>5005830.6</v>
       </c>
       <c r="H582" t="s">
         <v>11</v>
@@ -20358,19 +20329,19 @@
         <v>280</v>
       </c>
       <c r="B583">
-        <v>9019</v>
+        <v>9020</v>
       </c>
       <c r="C583" s="7">
-        <v>155.415584884957</v>
+        <v>151.630709636953</v>
       </c>
       <c r="D583" s="7">
-        <v>48.772</v>
+        <v>48.682</v>
       </c>
       <c r="E583" s="7">
-        <v>1427504.91</v>
+        <v>1427506.53</v>
       </c>
       <c r="F583" s="7">
-        <v>5005823.02</v>
+        <v>5005826.46</v>
       </c>
       <c r="H583" t="s">
         <v>11</v>
@@ -20387,19 +20358,19 @@
         <v>280</v>
       </c>
       <c r="B584">
-        <v>9018</v>
+        <v>9019</v>
       </c>
       <c r="C584" s="7">
-        <v>164.71386664454</v>
+        <v>155.415584884957</v>
       </c>
       <c r="D584" s="7">
-        <v>49.152</v>
+        <v>48.772</v>
       </c>
       <c r="E584" s="7">
-        <v>1427499.65</v>
+        <v>1427504.91</v>
       </c>
       <c r="F584" s="7">
-        <v>5005815.33</v>
+        <v>5005823.02</v>
       </c>
       <c r="H584" t="s">
         <v>11</v>
@@ -20416,19 +20387,19 @@
         <v>280</v>
       </c>
       <c r="B585">
-        <v>9017</v>
+        <v>9018</v>
       </c>
       <c r="C585" s="7">
-        <v>167.382156829968</v>
+        <v>164.71386664454</v>
       </c>
       <c r="D585" s="7">
-        <v>49.272</v>
+        <v>49.152</v>
       </c>
       <c r="E585" s="7">
-        <v>1427498.13</v>
+        <v>1427499.65</v>
       </c>
       <c r="F585" s="7">
-        <v>5005813.13</v>
+        <v>5005815.33</v>
       </c>
       <c r="H585" t="s">
         <v>11</v>
@@ -20445,19 +20416,19 @@
         <v>280</v>
       </c>
       <c r="B586">
-        <v>9016</v>
+        <v>9017</v>
       </c>
       <c r="C586" s="7">
-        <v>169.698567834418</v>
+        <v>167.382156829968</v>
       </c>
       <c r="D586" s="7">
-        <v>48.972</v>
+        <v>49.272</v>
       </c>
       <c r="E586" s="7">
-        <v>1427497.38</v>
+        <v>1427498.13</v>
       </c>
       <c r="F586" s="7">
-        <v>5005810.88</v>
+        <v>5005813.13</v>
       </c>
       <c r="H586" t="s">
         <v>11</v>
@@ -20474,19 +20445,19 @@
         <v>280</v>
       </c>
       <c r="B587">
-        <v>9015</v>
+        <v>9016</v>
       </c>
       <c r="C587" s="7">
-        <v>172.74858362669</v>
+        <v>169.698567834418</v>
       </c>
       <c r="D587" s="7">
-        <v>49.092</v>
+        <v>48.972</v>
       </c>
       <c r="E587" s="7">
-        <v>1427495.97</v>
+        <v>1427497.38</v>
       </c>
       <c r="F587" s="7">
-        <v>5005808.17</v>
+        <v>5005810.88</v>
       </c>
       <c r="H587" t="s">
         <v>11</v>
@@ -20503,19 +20474,19 @@
         <v>280</v>
       </c>
       <c r="B588">
-        <v>9014</v>
+        <v>9015</v>
       </c>
       <c r="C588" s="7">
-        <v>175.457933434288</v>
+        <v>172.74858362669</v>
       </c>
       <c r="D588" s="7">
-        <v>49.112</v>
+        <v>49.092</v>
       </c>
       <c r="E588" s="7">
-        <v>1427494.52</v>
+        <v>1427495.97</v>
       </c>
       <c r="F588" s="7">
-        <v>5005805.88</v>
+        <v>5005808.17</v>
       </c>
       <c r="H588" t="s">
         <v>11</v>
@@ -20532,19 +20503,19 @@
         <v>280</v>
       </c>
       <c r="B589">
-        <v>9013</v>
+        <v>9014</v>
       </c>
       <c r="C589" s="7">
-        <v>182.865446940821</v>
+        <v>175.457933434288</v>
       </c>
       <c r="D589" s="7">
-        <v>49.052</v>
+        <v>49.112</v>
       </c>
       <c r="E589" s="7">
-        <v>1427491.28</v>
+        <v>1427494.52</v>
       </c>
       <c r="F589" s="7">
-        <v>5005799.19</v>
+        <v>5005805.88</v>
       </c>
       <c r="H589" t="s">
         <v>11</v>
@@ -20561,19 +20532,19 @@
         <v>280</v>
       </c>
       <c r="B590">
-        <v>9012</v>
+        <v>9013</v>
       </c>
       <c r="C590" s="7">
-        <v>190.84340424833</v>
+        <v>182.865446940821</v>
       </c>
       <c r="D590" s="7">
-        <v>49.022</v>
+        <v>49.052</v>
       </c>
       <c r="E590" s="7">
-        <v>1427486.97</v>
+        <v>1427491.28</v>
       </c>
       <c r="F590" s="7">
-        <v>5005792.47</v>
+        <v>5005799.19</v>
       </c>
       <c r="H590" t="s">
         <v>11</v>
@@ -20590,19 +20561,19 @@
         <v>280</v>
       </c>
       <c r="B591">
-        <v>9011</v>
+        <v>9012</v>
       </c>
       <c r="C591" s="7">
-        <v>194.406738013259</v>
+        <v>190.84340424833</v>
       </c>
       <c r="D591" s="7">
-        <v>49.102</v>
+        <v>49.022</v>
       </c>
       <c r="E591" s="7">
-        <v>1427484.79</v>
+        <v>1427486.97</v>
       </c>
       <c r="F591" s="7">
-        <v>5005789.62</v>
+        <v>5005792.47</v>
       </c>
       <c r="H591" t="s">
         <v>11</v>
@@ -20619,19 +20590,19 @@
         <v>280</v>
       </c>
       <c r="B592">
-        <v>9010</v>
+        <v>9011</v>
       </c>
       <c r="C592" s="7">
-        <v>199.517046251427</v>
+        <v>194.406738013259</v>
       </c>
       <c r="D592" s="7">
         <v>49.102</v>
       </c>
       <c r="E592" s="7">
-        <v>1427482.09</v>
+        <v>1427484.79</v>
       </c>
       <c r="F592" s="7">
-        <v>5005785.28</v>
+        <v>5005789.62</v>
       </c>
       <c r="H592" t="s">
         <v>11</v>
@@ -20648,19 +20619,19 @@
         <v>280</v>
       </c>
       <c r="B593">
-        <v>9009</v>
+        <v>9010</v>
       </c>
       <c r="C593" s="7">
-        <v>201.759839078572</v>
+        <v>199.517046251427</v>
       </c>
       <c r="D593" s="7">
-        <v>49.282</v>
+        <v>49.102</v>
       </c>
       <c r="E593" s="7">
-        <v>1427480.83</v>
+        <v>1427482.09</v>
       </c>
       <c r="F593" s="7">
-        <v>5005783.42</v>
+        <v>5005785.28</v>
       </c>
       <c r="H593" t="s">
         <v>11</v>
@@ -20677,25 +20648,25 @@
         <v>280</v>
       </c>
       <c r="B594">
-        <v>9008</v>
+        <v>9009</v>
       </c>
       <c r="C594" s="7">
-        <v>205.600583717688</v>
+        <v>201.759839078572</v>
       </c>
       <c r="D594" s="7">
-        <v>49.122</v>
+        <v>49.282</v>
       </c>
       <c r="E594" s="7">
-        <v>1427478.43</v>
+        <v>1427480.83</v>
       </c>
       <c r="F594" s="7">
-        <v>5005780.38</v>
+        <v>5005783.42</v>
       </c>
       <c r="H594" t="s">
         <v>11</v>
       </c>
       <c r="I594" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K594" t="s">
         <v>281</v>
@@ -20706,25 +20677,25 @@
         <v>280</v>
       </c>
       <c r="B595">
-        <v>9007</v>
+        <v>9008</v>
       </c>
       <c r="C595" s="7">
-        <v>208.858048408852</v>
+        <v>205.600583717688</v>
       </c>
       <c r="D595" s="7">
-        <v>51.462</v>
+        <v>49.122</v>
       </c>
       <c r="E595" s="7">
-        <v>1427477.15</v>
+        <v>1427478.43</v>
       </c>
       <c r="F595" s="7">
-        <v>5005777.35</v>
+        <v>5005780.38</v>
       </c>
       <c r="H595" t="s">
         <v>11</v>
       </c>
       <c r="I595" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K595" t="s">
         <v>281</v>
@@ -20735,25 +20706,25 @@
         <v>280</v>
       </c>
       <c r="B596">
-        <v>9006</v>
+        <v>9007</v>
       </c>
       <c r="C596" s="7">
-        <v>209.323219507619</v>
+        <v>208.858048408852</v>
       </c>
       <c r="D596" s="7">
-        <v>51.312</v>
+        <v>51.462</v>
       </c>
       <c r="E596" s="7">
-        <v>1427477.03</v>
+        <v>1427477.15</v>
       </c>
       <c r="F596" s="7">
-        <v>5005776.88</v>
+        <v>5005777.35</v>
       </c>
       <c r="H596" t="s">
         <v>11</v>
       </c>
       <c r="I596" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="K596" t="s">
         <v>281</v>
@@ -20764,19 +20735,19 @@
         <v>280</v>
       </c>
       <c r="B597">
-        <v>9005</v>
+        <v>9006</v>
       </c>
       <c r="C597" s="7">
-        <v>211.1535191869</v>
+        <v>209.323219507619</v>
       </c>
       <c r="D597" s="7">
-        <v>51.392</v>
+        <v>51.312</v>
       </c>
       <c r="E597" s="7">
-        <v>1427476.19</v>
+        <v>1427477.03</v>
       </c>
       <c r="F597" s="7">
-        <v>5005775.25</v>
+        <v>5005776.88</v>
       </c>
       <c r="H597" t="s">
         <v>11</v>
@@ -20793,19 +20764,19 @@
         <v>280</v>
       </c>
       <c r="B598">
-        <v>9004</v>
+        <v>9005</v>
       </c>
       <c r="C598" s="7">
-        <v>215.490693731568</v>
+        <v>211.1535191869</v>
       </c>
       <c r="D598" s="7">
-        <v>51.422</v>
+        <v>51.392</v>
       </c>
       <c r="E598" s="7">
-        <v>1427473.96</v>
+        <v>1427476.19</v>
       </c>
       <c r="F598" s="7">
-        <v>5005771.53</v>
+        <v>5005775.25</v>
       </c>
       <c r="H598" t="s">
         <v>11</v>
@@ -20822,19 +20793,19 @@
         <v>280</v>
       </c>
       <c r="B599">
-        <v>9003</v>
+        <v>9004</v>
       </c>
       <c r="C599" s="7">
-        <v>222.434031715099</v>
+        <v>215.490693731568</v>
       </c>
       <c r="D599" s="7">
-        <v>51.692</v>
+        <v>51.422</v>
       </c>
       <c r="E599" s="7">
-        <v>1427470.23</v>
+        <v>1427473.96</v>
       </c>
       <c r="F599" s="7">
-        <v>5005765.67</v>
+        <v>5005771.53</v>
       </c>
       <c r="H599" t="s">
         <v>11</v>
@@ -20851,28 +20822,25 @@
         <v>280</v>
       </c>
       <c r="B600">
-        <v>9000</v>
+        <v>9003</v>
       </c>
       <c r="C600" s="7">
-        <v>225.712102610946</v>
+        <v>222.434031715099</v>
       </c>
       <c r="D600" s="7">
-        <v>51.882</v>
+        <v>51.692</v>
       </c>
       <c r="E600" s="7">
-        <v>1427470.27</v>
+        <v>1427470.23</v>
       </c>
       <c r="F600" s="7">
-        <v>5005761.84</v>
+        <v>5005765.67</v>
       </c>
       <c r="H600" t="s">
         <v>11</v>
       </c>
       <c r="I600" t="s">
-        <v>284</v>
-      </c>
-      <c r="J600" s="8" t="s">
-        <v>285</v>
+        <v>15</v>
       </c>
       <c r="K600" t="s">
         <v>281</v>
@@ -20883,25 +20851,28 @@
         <v>280</v>
       </c>
       <c r="B601">
-        <v>9002</v>
+        <v>9000</v>
       </c>
       <c r="C601" s="7">
-        <v>225.990823231784</v>
+        <v>225.712102610946</v>
       </c>
       <c r="D601" s="7">
-        <v>51.702</v>
+        <v>51.882</v>
       </c>
       <c r="E601" s="7">
-        <v>1427467.35</v>
+        <v>1427470.27</v>
       </c>
       <c r="F601" s="7">
-        <v>5005763.25</v>
+        <v>5005761.84</v>
       </c>
       <c r="H601" t="s">
         <v>11</v>
       </c>
       <c r="I601" t="s">
-        <v>131</v>
+        <v>284</v>
+      </c>
+      <c r="J601" s="8" t="s">
+        <v>285</v>
       </c>
       <c r="K601" t="s">
         <v>281</v>
@@ -20912,27 +20883,56 @@
         <v>280</v>
       </c>
       <c r="B602">
+        <v>9002</v>
+      </c>
+      <c r="C602" s="7">
+        <v>225.990823231784</v>
+      </c>
+      <c r="D602" s="7">
+        <v>51.702</v>
+      </c>
+      <c r="E602" s="7">
+        <v>1427467.35</v>
+      </c>
+      <c r="F602" s="7">
+        <v>5005763.25</v>
+      </c>
+      <c r="H602" t="s">
+        <v>11</v>
+      </c>
+      <c r="I602" t="s">
+        <v>131</v>
+      </c>
+      <c r="K602" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="603" spans="1:11">
+      <c r="A603" t="s">
+        <v>280</v>
+      </c>
+      <c r="B603">
         <v>9001</v>
       </c>
-      <c r="C602" s="7">
+      <c r="C603" s="7">
         <v>226.742936527025</v>
       </c>
-      <c r="D602" s="7">
+      <c r="D603" s="7">
         <v>51.772</v>
       </c>
-      <c r="E602" s="7">
+      <c r="E603" s="7">
         <v>1427467.57</v>
       </c>
-      <c r="F602" s="7">
+      <c r="F603" s="7">
         <v>5005762.24</v>
       </c>
-      <c r="H602" t="s">
-        <v>11</v>
-      </c>
-      <c r="I602" t="s">
-        <v>15</v>
-      </c>
-      <c r="K602" t="s">
+      <c r="H603" t="s">
+        <v>11</v>
+      </c>
+      <c r="I603" t="s">
+        <v>15</v>
+      </c>
+      <c r="K603" t="s">
         <v>281</v>
       </c>
     </row>

</xml_diff>